<commit_message>
Add EI_NDC scenario and update MCGLT to meet scenario demand
</commit_message>
<xml_diff>
--- a/InputData/elec/MCGLT/Max Cap Growth Lookup Table.xlsx
+++ b/InputData/elec/MCGLT/Max Cap Growth Lookup Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23258" windowHeight="12578"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23258" windowHeight="12578" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="43" r:id="rId1"/>
@@ -381,13 +381,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -425,7 +424,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -535,13 +533,13 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1650.0000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3000</c:v>
+                  <c:v>4950</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12000</c:v>
+                  <c:v>19800</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5000</c:v>
@@ -772,7 +770,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -853,7 +850,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1253,7 +1249,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1334,7 +1329,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1743,16 +1737,16 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2000</c:v>
+                  <c:v>3300.0000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2000</c:v>
+                  <c:v>3300.0000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6000</c:v>
+                  <c:v>9900</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1767,7 +1761,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6000</c:v>
+                  <c:v>9900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1899,7 +1893,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1980,7 +1973,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2155,28 +2147,28 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>500</c:v>
+                  <c:v>825.00000000000011</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>800</c:v>
+                  <c:v>1320</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>1650.0000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1500</c:v>
+                  <c:v>2475</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2000</c:v>
+                  <c:v>3300.0000000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2500</c:v>
+                  <c:v>4125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3000</c:v>
+                  <c:v>4950</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3500</c:v>
+                  <c:v>5775.0000000000009</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>3500</c:v>
@@ -5290,7 +5282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -5310,14 +5302,14 @@
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="3"/>
@@ -5335,14 +5327,14 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="3"/>
@@ -5354,15 +5346,15 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="3"/>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="30" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="29" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5372,40 +5364,40 @@
         <v>27</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="29" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="3"/>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="3"/>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="3"/>
-      <c r="B13" s="9"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="3"/>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="30" t="s">
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="29" t="s">
         <v>66</v>
       </c>
     </row>
@@ -5415,246 +5407,246 @@
         <v>65</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="H15" s="30" t="s">
+      <c r="H15" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="3"/>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="27" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="3"/>
-      <c r="B17" s="9"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="114" x14ac:dyDescent="0.45">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="114" x14ac:dyDescent="0.45">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="213.75" x14ac:dyDescent="0.45">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="24" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="24" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="24" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="171" x14ac:dyDescent="0.45">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="25"/>
+      <c r="C26" s="24"/>
     </row>
     <row r="27" spans="1:3" ht="114" x14ac:dyDescent="0.45">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="25">
+      <c r="B28" s="24">
         <v>0</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="24" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="24" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="114" x14ac:dyDescent="0.45">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="24" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="25"/>
+      <c r="C33" s="24"/>
     </row>
     <row r="34" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="24" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="57" x14ac:dyDescent="0.45">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="24" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A38" s="25"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A39" s="25"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A40" s="25"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A41" s="25"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
+      <c r="A41" s="24"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A42" s="25"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A43" s="25"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5674,8 +5666,8 @@
   </sheetPr>
   <dimension ref="A1:AS37"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:Y37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5693,364 +5685,437 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="7">
+      <c r="C1" s="6">
         <v>0</v>
       </c>
-      <c r="D1" s="7">
+      <c r="D1" s="6">
         <v>999999999999</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="12"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="11"/>
       <c r="M1" s="3"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="11">
-        <v>12000</v>
-      </c>
-      <c r="D2" s="11">
-        <v>12000</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="12"/>
+      <c r="C2" s="10">
+        <v>19800</v>
+      </c>
+      <c r="D2" s="10">
+        <v>19800</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="11"/>
       <c r="M2" s="3"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.45">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>0</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>999999999999</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="12"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="11"/>
       <c r="M3" s="3"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>2500</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>2500</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="12"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="11"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.45">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>0</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>999999999999</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="12"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="11"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>150</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>150</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="12"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="11"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
     </row>
     <row r="7" spans="1:45" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>0</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>50000</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>100000</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <v>150000</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="14">
         <v>200000</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>999999999999</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="7"/>
-      <c r="AC7" s="8"/>
-      <c r="AD7" s="8"/>
-      <c r="AE7" s="8"/>
-      <c r="AF7" s="8"/>
-      <c r="AG7" s="8"/>
-      <c r="AH7" s="8"/>
-      <c r="AI7" s="8"/>
-      <c r="AJ7" s="8"/>
-      <c r="AK7" s="8"/>
-      <c r="AL7" s="8"/>
-      <c r="AM7" s="8"/>
-      <c r="AN7" s="8"/>
-      <c r="AO7" s="8"/>
-      <c r="AP7" s="8"/>
-      <c r="AQ7" s="8"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
+      <c r="AK7" s="7"/>
+      <c r="AL7" s="7"/>
+      <c r="AM7" s="7"/>
+      <c r="AN7" s="7"/>
+      <c r="AO7" s="7"/>
+      <c r="AP7" s="7"/>
+      <c r="AQ7" s="7"/>
     </row>
     <row r="8" spans="1:45" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>2000</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>2000</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>1000</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>500</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>100</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <f>G8</f>
         <v>100</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="8"/>
-      <c r="AI8" s="8"/>
-      <c r="AJ8" s="8"/>
-      <c r="AK8" s="8"/>
-      <c r="AL8" s="8"/>
-      <c r="AM8" s="8"/>
-      <c r="AN8" s="8"/>
-      <c r="AO8" s="8"/>
-      <c r="AP8" s="8"/>
-      <c r="AQ8" s="8"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="7"/>
+      <c r="AL8" s="7"/>
+      <c r="AM8" s="7"/>
+      <c r="AN8" s="7"/>
+      <c r="AO8" s="7"/>
+      <c r="AP8" s="7"/>
+      <c r="AQ8" s="7"/>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.45">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>0</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>12000</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>20000</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>40000</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>999999999999</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
       <c r="AS9" s="4"/>
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.45">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="11">
-        <v>2000</v>
-      </c>
-      <c r="D10" s="11">
-        <v>2000</v>
-      </c>
-      <c r="E10" s="11">
-        <v>4000</v>
-      </c>
-      <c r="F10" s="11">
+      <c r="C10" s="10">
+        <v>3300.0000000000005</v>
+      </c>
+      <c r="D10" s="10">
+        <v>3300.0000000000005</v>
+      </c>
+      <c r="E10" s="10">
+        <v>6600.0000000000009</v>
+      </c>
+      <c r="F10" s="10">
+        <v>9900</v>
+      </c>
+      <c r="G10" s="10">
+        <v>9900</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.45">
+      <c r="A11" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>3000</v>
+      </c>
+      <c r="E11" s="6">
         <v>6000</v>
       </c>
-      <c r="G10" s="11">
-        <v>6000</v>
-      </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.45">
-      <c r="A11" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="7">
-        <v>0</v>
-      </c>
-      <c r="D11" s="7">
-        <v>3000</v>
-      </c>
-      <c r="E11" s="7">
-        <v>6000</v>
-      </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>20000</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>999999999999</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="5"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="16"/>
       <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
       <c r="AA11" s="4"/>
@@ -6073,605 +6138,802 @@
       <c r="AR11" s="4"/>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.45">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
+        <v>1650.0000000000002</v>
+      </c>
+      <c r="D12" s="6">
+        <v>4950</v>
+      </c>
+      <c r="E12" s="6">
+        <v>9900</v>
+      </c>
+      <c r="F12" s="6">
+        <v>19800</v>
+      </c>
+      <c r="G12" s="6">
+        <v>19800</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6"/>
+      <c r="AE12" s="6"/>
+      <c r="AF12" s="6"/>
+      <c r="AG12" s="6"/>
+      <c r="AH12" s="6"/>
+      <c r="AI12" s="6"/>
+      <c r="AJ12" s="6"/>
+      <c r="AK12" s="6"/>
+      <c r="AL12" s="6"/>
+      <c r="AM12" s="6"/>
+      <c r="AN12" s="6"/>
+      <c r="AO12" s="6"/>
+      <c r="AP12" s="6"/>
+      <c r="AQ12" s="6"/>
+      <c r="AR12" s="6"/>
+      <c r="AS12" s="6"/>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.45">
+      <c r="A13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="14">
+        <v>0</v>
+      </c>
+      <c r="D13" s="14">
+        <v>500</v>
+      </c>
+      <c r="E13" s="14">
         <v>1000</v>
       </c>
-      <c r="D12" s="7">
-        <v>3000</v>
-      </c>
-      <c r="E12" s="7">
-        <v>6000</v>
-      </c>
-      <c r="F12" s="7">
-        <v>12000</v>
-      </c>
-      <c r="G12" s="7">
-        <v>12000</v>
-      </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="7"/>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="7"/>
-      <c r="AC12" s="7"/>
-      <c r="AD12" s="7"/>
-      <c r="AE12" s="7"/>
-      <c r="AF12" s="7"/>
-      <c r="AG12" s="7"/>
-      <c r="AH12" s="7"/>
-      <c r="AI12" s="7"/>
-      <c r="AJ12" s="7"/>
-      <c r="AK12" s="7"/>
-      <c r="AL12" s="7"/>
-      <c r="AM12" s="7"/>
-      <c r="AN12" s="7"/>
-      <c r="AO12" s="7"/>
-      <c r="AP12" s="7"/>
-      <c r="AQ12" s="7"/>
-      <c r="AR12" s="7"/>
-      <c r="AS12" s="7"/>
-    </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.45">
-      <c r="A13" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="17" t="s">
+      <c r="F13" s="14">
+        <v>1500</v>
+      </c>
+      <c r="G13" s="14">
+        <v>2000</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="7"/>
+      <c r="AI13" s="7"/>
+      <c r="AJ13" s="7"/>
+      <c r="AK13" s="7"/>
+      <c r="AL13" s="7"/>
+      <c r="AM13" s="7"/>
+      <c r="AN13" s="7"/>
+      <c r="AO13" s="7"/>
+      <c r="AP13" s="7"/>
+      <c r="AQ13" s="7"/>
+      <c r="AR13" s="7"/>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.45">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="10">
+        <v>50</v>
+      </c>
+      <c r="D14" s="10">
+        <v>100</v>
+      </c>
+      <c r="E14" s="10">
+        <v>200</v>
+      </c>
+      <c r="F14" s="10">
+        <v>400</v>
+      </c>
+      <c r="G14" s="10">
+        <v>800</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.45">
+      <c r="A15" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C15" s="18">
         <v>0</v>
       </c>
-      <c r="D13" s="15">
-        <v>500</v>
-      </c>
-      <c r="E13" s="15">
-        <v>1000</v>
-      </c>
-      <c r="F13" s="15">
-        <v>1500</v>
-      </c>
-      <c r="G13" s="15">
-        <v>2000</v>
-      </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
-      <c r="AC13" s="8"/>
-      <c r="AD13" s="8"/>
-      <c r="AE13" s="8"/>
-      <c r="AF13" s="8"/>
-      <c r="AG13" s="8"/>
-      <c r="AH13" s="8"/>
-      <c r="AI13" s="8"/>
-      <c r="AJ13" s="8"/>
-      <c r="AK13" s="8"/>
-      <c r="AL13" s="8"/>
-      <c r="AM13" s="8"/>
-      <c r="AN13" s="8"/>
-      <c r="AO13" s="8"/>
-      <c r="AP13" s="8"/>
-      <c r="AQ13" s="8"/>
-      <c r="AR13" s="8"/>
-    </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.45">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18" t="s">
+      <c r="D15" s="18">
+        <v>999999999</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.45">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="11">
-        <v>50</v>
-      </c>
-      <c r="D14" s="11">
-        <v>100</v>
-      </c>
-      <c r="E14" s="11">
-        <v>200</v>
-      </c>
-      <c r="F14" s="11">
+      <c r="C16" s="20">
         <v>400</v>
       </c>
-      <c r="G14" s="11">
-        <v>800</v>
-      </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-    </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.45">
-      <c r="A15" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="17" t="s">
+      <c r="D16" s="20">
+        <v>400</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C17" s="19">
         <v>0</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D17" s="19">
         <v>999999999</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.45">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18" t="s">
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="21">
-        <v>400</v>
-      </c>
-      <c r="D16" s="21">
-        <v>400</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="3"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A17" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="17" t="s">
+      <c r="C18" s="20">
+        <v>0</v>
+      </c>
+      <c r="D18" s="20">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C19" s="14">
         <v>0</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D19" s="14">
         <v>999999999</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="21">
-        <v>0</v>
-      </c>
-      <c r="D18" s="21">
-        <v>0</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="15">
-        <v>0</v>
-      </c>
-      <c r="D19" s="15">
-        <v>999999999</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="10">
         <v>100</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="10">
         <v>100</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A21" s="6" t="s">
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="21">
         <v>0</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="21">
         <v>999999999</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="23">
+      <c r="C22" s="22">
         <v>1500</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="22">
         <v>1500</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A23" s="6" t="s">
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="14">
         <v>0</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="14">
         <v>999999999</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="10">
+        <v>18000</v>
+      </c>
+      <c r="D24" s="10">
+        <v>18000</v>
+      </c>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="14">
+        <v>0</v>
+      </c>
+      <c r="D25" s="14">
+        <v>3000</v>
+      </c>
+      <c r="E25" s="14">
+        <v>6000</v>
+      </c>
+      <c r="F25" s="14">
+        <v>9000</v>
+      </c>
+      <c r="G25" s="14">
         <v>12000</v>
       </c>
-      <c r="D24" s="11">
-        <v>12000</v>
-      </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="15">
-        <v>0</v>
-      </c>
-      <c r="D25" s="15">
-        <v>3000</v>
-      </c>
-      <c r="E25" s="15">
-        <v>6000</v>
-      </c>
-      <c r="F25" s="15">
-        <v>9000</v>
-      </c>
-      <c r="G25" s="15">
-        <v>12000</v>
-      </c>
-      <c r="H25" s="15">
+      <c r="H25" s="14">
         <v>15000</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="14">
         <v>18000</v>
       </c>
-      <c r="J25" s="15">
+      <c r="J25" s="14">
         <v>21000</v>
       </c>
-      <c r="K25" s="15">
+      <c r="K25" s="14">
         <v>24000</v>
       </c>
-      <c r="L25" s="12"/>
+      <c r="L25" s="11"/>
       <c r="M25" s="3"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="11">
-        <v>500</v>
-      </c>
-      <c r="D26" s="11">
-        <v>800</v>
-      </c>
-      <c r="E26" s="11">
-        <v>1000</v>
-      </c>
-      <c r="F26" s="11">
-        <v>1500</v>
-      </c>
-      <c r="G26" s="11">
-        <v>2000</v>
-      </c>
-      <c r="H26" s="11">
-        <v>2500</v>
-      </c>
-      <c r="I26" s="11">
-        <v>3000</v>
-      </c>
-      <c r="J26" s="11">
-        <v>3500</v>
-      </c>
-      <c r="K26" s="11">
-        <v>4000</v>
-      </c>
-      <c r="L26" s="12"/>
+      <c r="C26" s="10">
+        <v>825.00000000000011</v>
+      </c>
+      <c r="D26" s="10">
+        <v>1320</v>
+      </c>
+      <c r="E26" s="10">
+        <v>1650.0000000000002</v>
+      </c>
+      <c r="F26" s="10">
+        <v>2475</v>
+      </c>
+      <c r="G26" s="10">
+        <v>3300.0000000000005</v>
+      </c>
+      <c r="H26" s="10">
+        <v>4125</v>
+      </c>
+      <c r="I26" s="10">
+        <v>4950</v>
+      </c>
+      <c r="J26" s="10">
+        <v>5775.0000000000009</v>
+      </c>
+      <c r="K26" s="10">
+        <v>6600.0000000000009</v>
+      </c>
+      <c r="L26" s="11"/>
       <c r="M26" s="3"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A27" s="6" t="s">
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="14">
         <v>0</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="14">
         <v>999999999</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="12"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="11"/>
       <c r="M27" s="3"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="10">
         <v>100</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="10">
         <v>100</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="12"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="11"/>
       <c r="M28" s="3"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A29" s="6" t="s">
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A29" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="14">
         <v>0</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="14">
         <v>999999999</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="12"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="11"/>
       <c r="M29" s="3"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="6"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="10">
         <v>300</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="10">
         <v>300</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="12"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="11"/>
       <c r="M30" s="3"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A31" s="6" t="s">
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="6"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A31" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="14">
         <v>0</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="14">
         <v>500</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="14">
         <v>1000</v>
       </c>
-      <c r="F31" s="15">
+      <c r="F31" s="14">
         <v>1500</v>
       </c>
-      <c r="G31" s="15">
+      <c r="G31" s="14">
         <v>2000</v>
       </c>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="12"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="11"/>
       <c r="M31" s="3"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
+      <c r="U31" s="6"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="6"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="10">
         <v>50</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="10">
         <v>100</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="10">
         <v>200</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="10">
         <v>400</v>
       </c>
-      <c r="G32" s="11">
+      <c r="G32" s="10">
         <v>800</v>
       </c>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="12"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="11"/>
       <c r="M32" s="3"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="6"/>
+      <c r="U32" s="6"/>
+      <c r="V32" s="6"/>
+      <c r="W32" s="6"/>
+      <c r="X32" s="6"/>
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
       <c r="M33" s="3"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
       <c r="M34" s="3"/>
     </row>
     <row r="35" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
     </row>
     <row r="37" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6698,40 +6960,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.45">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="12"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="11"/>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.45">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="12"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.45">
-      <c r="A3" s="7"/>
-      <c r="B3" s="29" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>0</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>3000</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>6000</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>9000</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>12000</v>
       </c>
-      <c r="I3" s="29" t="s">
+      <c r="I3" s="28" t="s">
         <v>55</v>
       </c>
       <c r="J3" s="4">
@@ -6755,7 +7017,7 @@
         <v>2000</v>
       </c>
       <c r="O3" s="4"/>
-      <c r="P3" s="29" t="s">
+      <c r="P3" s="28" t="s">
         <v>58</v>
       </c>
       <c r="Q3" s="4">
@@ -6787,7 +7049,7 @@
         <v>24000</v>
       </c>
       <c r="Z3" s="4"/>
-      <c r="AA3" s="29" t="s">
+      <c r="AA3" s="28" t="s">
         <v>59</v>
       </c>
       <c r="AB3" s="4">
@@ -6828,29 +7090,29 @@
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.45">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <f>MCGLT!C12</f>
-        <v>1000</v>
-      </c>
-      <c r="D4" s="7">
+        <v>1650.0000000000002</v>
+      </c>
+      <c r="D4" s="6">
         <f>MCGLT!D12</f>
-        <v>3000</v>
-      </c>
-      <c r="E4" s="7">
+        <v>4950</v>
+      </c>
+      <c r="E4" s="6">
         <f>MCGLT!F12</f>
-        <v>12000</v>
-      </c>
-      <c r="F4" s="7">
+        <v>19800</v>
+      </c>
+      <c r="F4" s="6">
         <v>5000</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>8000</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>57</v>
       </c>
       <c r="J4" s="4">
@@ -6874,7 +7136,7 @@
         <v>800</v>
       </c>
       <c r="O4" s="4"/>
-      <c r="P4" s="7" t="s">
+      <c r="P4" s="6" t="s">
         <v>71</v>
       </c>
       <c r="Q4" s="4">
@@ -6904,156 +7166,156 @@
       <c r="Y4" s="4">
         <v>600</v>
       </c>
-      <c r="AA4" s="7" t="s">
+      <c r="AA4" s="6" t="s">
         <v>60</v>
       </c>
       <c r="AB4" s="4">
         <f>MCGLT!C26</f>
-        <v>500</v>
+        <v>825.00000000000011</v>
       </c>
       <c r="AC4" s="4">
         <f>MCGLT!D26</f>
-        <v>800</v>
+        <v>1320</v>
       </c>
       <c r="AD4" s="4">
         <f>MCGLT!E26</f>
-        <v>1000</v>
+        <v>1650.0000000000002</v>
       </c>
       <c r="AE4" s="4">
         <f>MCGLT!F26</f>
-        <v>1500</v>
+        <v>2475</v>
       </c>
       <c r="AF4" s="4">
         <f>MCGLT!G26</f>
-        <v>2000</v>
+        <v>3300.0000000000005</v>
       </c>
       <c r="AG4" s="4">
         <f>MCGLT!H26</f>
-        <v>2500</v>
+        <v>4125</v>
       </c>
       <c r="AH4" s="4">
         <f>MCGLT!I26</f>
-        <v>3000</v>
+        <v>4950</v>
       </c>
       <c r="AI4" s="4">
         <f>MCGLT!J26</f>
-        <v>3500</v>
+        <v>5775.0000000000009</v>
       </c>
       <c r="AJ4" s="4">
         <v>3500</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.45">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>1000</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>1000</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>1000</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>1000</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>1000</v>
       </c>
       <c r="I5" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="6">
         <v>0</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <v>0</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="6">
         <v>0</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="6">
         <v>0</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="6">
         <v>0</v>
       </c>
       <c r="P5" t="s">
         <v>53</v>
       </c>
-      <c r="Q5" s="7">
+      <c r="Q5" s="6">
         <v>2000</v>
       </c>
-      <c r="R5" s="7">
+      <c r="R5" s="6">
         <v>2000</v>
       </c>
-      <c r="S5" s="7">
+      <c r="S5" s="6">
         <v>2000</v>
       </c>
-      <c r="T5" s="7">
+      <c r="T5" s="6">
         <v>2000</v>
       </c>
-      <c r="U5" s="7">
+      <c r="U5" s="6">
         <v>2000</v>
       </c>
-      <c r="V5" s="7">
+      <c r="V5" s="6">
         <v>2000</v>
       </c>
-      <c r="W5" s="7">
+      <c r="W5" s="6">
         <v>2000</v>
       </c>
-      <c r="X5" s="7">
+      <c r="X5" s="6">
         <v>2000</v>
       </c>
-      <c r="Y5" s="7">
+      <c r="Y5" s="6">
         <v>2000</v>
       </c>
       <c r="AA5" t="s">
         <v>53</v>
       </c>
-      <c r="AB5" s="7">
+      <c r="AB5" s="6">
         <v>0</v>
       </c>
-      <c r="AC5" s="7">
+      <c r="AC5" s="6">
         <v>0</v>
       </c>
-      <c r="AD5" s="7">
+      <c r="AD5" s="6">
         <v>0</v>
       </c>
-      <c r="AE5" s="7">
+      <c r="AE5" s="6">
         <v>0</v>
       </c>
-      <c r="AF5" s="7">
+      <c r="AF5" s="6">
         <v>0</v>
       </c>
-      <c r="AG5" s="7">
+      <c r="AG5" s="6">
         <v>0</v>
       </c>
-      <c r="AH5" s="7">
+      <c r="AH5" s="6">
         <v>0</v>
       </c>
-      <c r="AI5" s="7">
+      <c r="AI5" s="6">
         <v>0</v>
       </c>
-      <c r="AJ5" s="7">
+      <c r="AJ5" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.45">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="12"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="3"/>
-      <c r="P6" s="7" t="s">
+      <c r="P6" s="6" t="s">
         <v>72</v>
       </c>
       <c r="Q6" s="4">
         <f>MCGLT!C10</f>
-        <v>2000</v>
+        <v>3300.0000000000005</v>
       </c>
       <c r="R6" s="4" t="e">
         <f>MCGLT!#REF!</f>
@@ -7061,11 +7323,11 @@
       </c>
       <c r="S6" s="4">
         <f>MCGLT!D10</f>
-        <v>2000</v>
+        <v>3300.0000000000005</v>
       </c>
       <c r="T6" s="4">
         <f>MCGLT!F10</f>
-        <v>6000</v>
+        <v>9900</v>
       </c>
       <c r="U6" s="4" t="e">
         <f>MCGLT!#REF!</f>
@@ -7085,77 +7347,77 @@
       </c>
       <c r="Y6" s="4">
         <f>MCGLT!G10</f>
-        <v>6000</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.45">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="12"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.45">
-      <c r="A8" s="16"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="12"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="3"/>
     </row>
     <row r="23" spans="2:29" x14ac:dyDescent="0.45">
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="J23" s="32" t="s">
+      <c r="C23" s="31"/>
+      <c r="J23" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="K23" s="33"/>
+      <c r="K23" s="31"/>
     </row>
     <row r="24" spans="2:29" x14ac:dyDescent="0.45">
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="J24" s="33" t="s">
+      <c r="C24" s="31"/>
+      <c r="J24" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="K24" s="33"/>
-      <c r="Q24" s="32" t="s">
+      <c r="K24" s="31"/>
+      <c r="Q24" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="R24" s="33"/>
+      <c r="R24" s="31"/>
     </row>
     <row r="25" spans="2:29" x14ac:dyDescent="0.45">
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="J25" s="33" t="s">
+      <c r="C25" s="31"/>
+      <c r="J25" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="K25" s="33"/>
-      <c r="Q25" s="33" t="s">
+      <c r="K25" s="31"/>
+      <c r="Q25" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="R25" s="33"/>
-      <c r="AB25" s="32" t="s">
+      <c r="R25" s="31"/>
+      <c r="AB25" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="AC25" s="33"/>
+      <c r="AC25" s="31"/>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>83</v>
       </c>
-      <c r="Q26" s="33" t="s">
+      <c r="Q26" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="R26" s="33"/>
-      <c r="AB26" s="33" t="s">
+      <c r="R26" s="31"/>
+      <c r="AB26" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="AC26" s="33"/>
+      <c r="AC26" s="31"/>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.45">
       <c r="P27" s="3"/>
@@ -7164,10 +7426,10 @@
       </c>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
-      <c r="AB27" s="33" t="s">
+      <c r="AB27" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="AC27" s="33"/>
+      <c r="AC27" s="31"/>
     </row>
     <row r="28" spans="2:29" x14ac:dyDescent="0.45">
       <c r="P28" s="3"/>

</xml_diff>